<commit_message>
Added Systems applicability table and style
</commit_message>
<xml_diff>
--- a/System 1 Patches.xlsx
+++ b/System 1 Patches.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,6 +548,97 @@
           <t>Comment</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr"/>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2016 Classic 6.98 McAfee</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2016 Classic 6.98 Symantec</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2019 Classic 6.97 McAfee</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2019 Classic 6.97 Symantec</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2016 Evo 24.1 McAfee</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2016 Evo 24.1 Symantec</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2016 Evo 24.1 Windows Defender</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2019 Evo 23.1 McAfee</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2019 Evo 23.1 Symantec</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2019 Evo 23.2 McAfee</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2019 Evo 23.2 Symantec</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2019 Evo 23.2 Windows Defender</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2022 Evo 22.2 McAfee</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Server 2022 Evo 22.2 Symantec</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Wind10 21H2 Classic 6.98 Evo versions: 22.X - 23.1</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Win10 22H2 Classic 6.97 Evo 23.2</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Win11 22H2 Evo 23.1</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Win11 23H2 Evo 24.1</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="46.5" customHeight="1">
       <c r="A2" s="2" t="n">
@@ -596,6 +687,25 @@
       <c r="J2" s="2" t="inlineStr"/>
       <c r="K2" s="2" t="inlineStr"/>
       <c r="L2" s="2" t="inlineStr"/>
+      <c r="M2" s="2" t="inlineStr"/>
+      <c r="N2" s="2" t="inlineStr"/>
+      <c r="O2" s="2" t="inlineStr"/>
+      <c r="P2" s="2" t="inlineStr"/>
+      <c r="Q2" s="2" t="inlineStr"/>
+      <c r="R2" s="2" t="inlineStr"/>
+      <c r="S2" s="2" t="inlineStr"/>
+      <c r="T2" s="2" t="inlineStr"/>
+      <c r="U2" s="2" t="inlineStr"/>
+      <c r="V2" s="2" t="inlineStr"/>
+      <c r="W2" s="2" t="inlineStr"/>
+      <c r="X2" s="2" t="inlineStr"/>
+      <c r="Y2" s="2" t="inlineStr"/>
+      <c r="Z2" s="2" t="inlineStr"/>
+      <c r="AA2" s="2" t="inlineStr"/>
+      <c r="AB2" s="2" t="inlineStr"/>
+      <c r="AC2" s="2" t="inlineStr"/>
+      <c r="AD2" s="2" t="inlineStr"/>
+      <c r="AE2" s="2" t="inlineStr"/>
     </row>
     <row r="3" ht="34.5" customHeight="1">
       <c r="A3" s="2" t="n">
@@ -644,6 +754,25 @@
       <c r="J3" s="2" t="inlineStr"/>
       <c r="K3" s="2" t="inlineStr"/>
       <c r="L3" s="2" t="inlineStr"/>
+      <c r="M3" s="2" t="inlineStr"/>
+      <c r="N3" s="2" t="inlineStr"/>
+      <c r="O3" s="2" t="inlineStr"/>
+      <c r="P3" s="2" t="inlineStr"/>
+      <c r="Q3" s="2" t="inlineStr"/>
+      <c r="R3" s="2" t="inlineStr"/>
+      <c r="S3" s="2" t="inlineStr"/>
+      <c r="T3" s="2" t="inlineStr"/>
+      <c r="U3" s="2" t="inlineStr"/>
+      <c r="V3" s="2" t="inlineStr"/>
+      <c r="W3" s="2" t="inlineStr"/>
+      <c r="X3" s="2" t="inlineStr"/>
+      <c r="Y3" s="2" t="inlineStr"/>
+      <c r="Z3" s="2" t="inlineStr"/>
+      <c r="AA3" s="2" t="inlineStr"/>
+      <c r="AB3" s="2" t="inlineStr"/>
+      <c r="AC3" s="2" t="inlineStr"/>
+      <c r="AD3" s="2" t="inlineStr"/>
+      <c r="AE3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -692,6 +821,25 @@
       <c r="J4" s="2" t="inlineStr"/>
       <c r="K4" s="2" t="inlineStr"/>
       <c r="L4" s="2" t="inlineStr"/>
+      <c r="M4" s="2" t="inlineStr"/>
+      <c r="N4" s="2" t="inlineStr"/>
+      <c r="O4" s="2" t="inlineStr"/>
+      <c r="P4" s="2" t="inlineStr"/>
+      <c r="Q4" s="2" t="inlineStr"/>
+      <c r="R4" s="2" t="inlineStr"/>
+      <c r="S4" s="2" t="inlineStr"/>
+      <c r="T4" s="2" t="inlineStr"/>
+      <c r="U4" s="2" t="inlineStr"/>
+      <c r="V4" s="2" t="inlineStr"/>
+      <c r="W4" s="2" t="inlineStr"/>
+      <c r="X4" s="2" t="inlineStr"/>
+      <c r="Y4" s="2" t="inlineStr"/>
+      <c r="Z4" s="2" t="inlineStr"/>
+      <c r="AA4" s="2" t="inlineStr"/>
+      <c r="AB4" s="2" t="inlineStr"/>
+      <c r="AC4" s="2" t="inlineStr"/>
+      <c r="AD4" s="2" t="inlineStr"/>
+      <c r="AE4" s="2" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -740,6 +888,25 @@
       <c r="J5" s="2" t="inlineStr"/>
       <c r="K5" s="2" t="inlineStr"/>
       <c r="L5" s="2" t="inlineStr"/>
+      <c r="M5" s="2" t="inlineStr"/>
+      <c r="N5" s="2" t="inlineStr"/>
+      <c r="O5" s="2" t="inlineStr"/>
+      <c r="P5" s="2" t="inlineStr"/>
+      <c r="Q5" s="2" t="inlineStr"/>
+      <c r="R5" s="2" t="inlineStr"/>
+      <c r="S5" s="2" t="inlineStr"/>
+      <c r="T5" s="2" t="inlineStr"/>
+      <c r="U5" s="2" t="inlineStr"/>
+      <c r="V5" s="2" t="inlineStr"/>
+      <c r="W5" s="2" t="inlineStr"/>
+      <c r="X5" s="2" t="inlineStr"/>
+      <c r="Y5" s="2" t="inlineStr"/>
+      <c r="Z5" s="2" t="inlineStr"/>
+      <c r="AA5" s="2" t="inlineStr"/>
+      <c r="AB5" s="2" t="inlineStr"/>
+      <c r="AC5" s="2" t="inlineStr"/>
+      <c r="AD5" s="2" t="inlineStr"/>
+      <c r="AE5" s="2" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -788,6 +955,25 @@
       <c r="J6" s="2" t="inlineStr"/>
       <c r="K6" s="2" t="inlineStr"/>
       <c r="L6" s="2" t="inlineStr"/>
+      <c r="M6" s="2" t="inlineStr"/>
+      <c r="N6" s="2" t="inlineStr"/>
+      <c r="O6" s="2" t="inlineStr"/>
+      <c r="P6" s="2" t="inlineStr"/>
+      <c r="Q6" s="2" t="inlineStr"/>
+      <c r="R6" s="2" t="inlineStr"/>
+      <c r="S6" s="2" t="inlineStr"/>
+      <c r="T6" s="2" t="inlineStr"/>
+      <c r="U6" s="2" t="inlineStr"/>
+      <c r="V6" s="2" t="inlineStr"/>
+      <c r="W6" s="2" t="inlineStr"/>
+      <c r="X6" s="2" t="inlineStr"/>
+      <c r="Y6" s="2" t="inlineStr"/>
+      <c r="Z6" s="2" t="inlineStr"/>
+      <c r="AA6" s="2" t="inlineStr"/>
+      <c r="AB6" s="2" t="inlineStr"/>
+      <c r="AC6" s="2" t="inlineStr"/>
+      <c r="AD6" s="2" t="inlineStr"/>
+      <c r="AE6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -836,6 +1022,25 @@
       <c r="J7" s="2" t="inlineStr"/>
       <c r="K7" s="2" t="inlineStr"/>
       <c r="L7" s="2" t="inlineStr"/>
+      <c r="M7" s="2" t="inlineStr"/>
+      <c r="N7" s="2" t="inlineStr"/>
+      <c r="O7" s="2" t="inlineStr"/>
+      <c r="P7" s="2" t="inlineStr"/>
+      <c r="Q7" s="2" t="inlineStr"/>
+      <c r="R7" s="2" t="inlineStr"/>
+      <c r="S7" s="2" t="inlineStr"/>
+      <c r="T7" s="2" t="inlineStr"/>
+      <c r="U7" s="2" t="inlineStr"/>
+      <c r="V7" s="2" t="inlineStr"/>
+      <c r="W7" s="2" t="inlineStr"/>
+      <c r="X7" s="2" t="inlineStr"/>
+      <c r="Y7" s="2" t="inlineStr"/>
+      <c r="Z7" s="2" t="inlineStr"/>
+      <c r="AA7" s="2" t="inlineStr"/>
+      <c r="AB7" s="2" t="inlineStr"/>
+      <c r="AC7" s="2" t="inlineStr"/>
+      <c r="AD7" s="2" t="inlineStr"/>
+      <c r="AE7" s="2" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -884,6 +1089,25 @@
       <c r="J8" s="2" t="inlineStr"/>
       <c r="K8" s="2" t="inlineStr"/>
       <c r="L8" s="2" t="inlineStr"/>
+      <c r="M8" s="2" t="inlineStr"/>
+      <c r="N8" s="2" t="inlineStr"/>
+      <c r="O8" s="2" t="inlineStr"/>
+      <c r="P8" s="2" t="inlineStr"/>
+      <c r="Q8" s="2" t="inlineStr"/>
+      <c r="R8" s="2" t="inlineStr"/>
+      <c r="S8" s="2" t="inlineStr"/>
+      <c r="T8" s="2" t="inlineStr"/>
+      <c r="U8" s="2" t="inlineStr"/>
+      <c r="V8" s="2" t="inlineStr"/>
+      <c r="W8" s="2" t="inlineStr"/>
+      <c r="X8" s="2" t="inlineStr"/>
+      <c r="Y8" s="2" t="inlineStr"/>
+      <c r="Z8" s="2" t="inlineStr"/>
+      <c r="AA8" s="2" t="inlineStr"/>
+      <c r="AB8" s="2" t="inlineStr"/>
+      <c r="AC8" s="2" t="inlineStr"/>
+      <c r="AD8" s="2" t="inlineStr"/>
+      <c r="AE8" s="2" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -932,6 +1156,25 @@
       <c r="J9" s="2" t="inlineStr"/>
       <c r="K9" s="2" t="inlineStr"/>
       <c r="L9" s="2" t="inlineStr"/>
+      <c r="M9" s="2" t="inlineStr"/>
+      <c r="N9" s="2" t="inlineStr"/>
+      <c r="O9" s="2" t="inlineStr"/>
+      <c r="P9" s="2" t="inlineStr"/>
+      <c r="Q9" s="2" t="inlineStr"/>
+      <c r="R9" s="2" t="inlineStr"/>
+      <c r="S9" s="2" t="inlineStr"/>
+      <c r="T9" s="2" t="inlineStr"/>
+      <c r="U9" s="2" t="inlineStr"/>
+      <c r="V9" s="2" t="inlineStr"/>
+      <c r="W9" s="2" t="inlineStr"/>
+      <c r="X9" s="2" t="inlineStr"/>
+      <c r="Y9" s="2" t="inlineStr"/>
+      <c r="Z9" s="2" t="inlineStr"/>
+      <c r="AA9" s="2" t="inlineStr"/>
+      <c r="AB9" s="2" t="inlineStr"/>
+      <c r="AC9" s="2" t="inlineStr"/>
+      <c r="AD9" s="2" t="inlineStr"/>
+      <c r="AE9" s="2" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -980,6 +1223,25 @@
       <c r="J10" s="2" t="inlineStr"/>
       <c r="K10" s="2" t="inlineStr"/>
       <c r="L10" s="2" t="inlineStr"/>
+      <c r="M10" s="2" t="inlineStr"/>
+      <c r="N10" s="2" t="inlineStr"/>
+      <c r="O10" s="2" t="inlineStr"/>
+      <c r="P10" s="2" t="inlineStr"/>
+      <c r="Q10" s="2" t="inlineStr"/>
+      <c r="R10" s="2" t="inlineStr"/>
+      <c r="S10" s="2" t="inlineStr"/>
+      <c r="T10" s="2" t="inlineStr"/>
+      <c r="U10" s="2" t="inlineStr"/>
+      <c r="V10" s="2" t="inlineStr"/>
+      <c r="W10" s="2" t="inlineStr"/>
+      <c r="X10" s="2" t="inlineStr"/>
+      <c r="Y10" s="2" t="inlineStr"/>
+      <c r="Z10" s="2" t="inlineStr"/>
+      <c r="AA10" s="2" t="inlineStr"/>
+      <c r="AB10" s="2" t="inlineStr"/>
+      <c r="AC10" s="2" t="inlineStr"/>
+      <c r="AD10" s="2" t="inlineStr"/>
+      <c r="AE10" s="2" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1028,6 +1290,25 @@
       <c r="J11" s="2" t="inlineStr"/>
       <c r="K11" s="2" t="inlineStr"/>
       <c r="L11" s="2" t="inlineStr"/>
+      <c r="M11" s="2" t="inlineStr"/>
+      <c r="N11" s="2" t="inlineStr"/>
+      <c r="O11" s="2" t="inlineStr"/>
+      <c r="P11" s="2" t="inlineStr"/>
+      <c r="Q11" s="2" t="inlineStr"/>
+      <c r="R11" s="2" t="inlineStr"/>
+      <c r="S11" s="2" t="inlineStr"/>
+      <c r="T11" s="2" t="inlineStr"/>
+      <c r="U11" s="2" t="inlineStr"/>
+      <c r="V11" s="2" t="inlineStr"/>
+      <c r="W11" s="2" t="inlineStr"/>
+      <c r="X11" s="2" t="inlineStr"/>
+      <c r="Y11" s="2" t="inlineStr"/>
+      <c r="Z11" s="2" t="inlineStr"/>
+      <c r="AA11" s="2" t="inlineStr"/>
+      <c r="AB11" s="2" t="inlineStr"/>
+      <c r="AC11" s="2" t="inlineStr"/>
+      <c r="AD11" s="2" t="inlineStr"/>
+      <c r="AE11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1076,6 +1357,25 @@
       <c r="J12" s="2" t="inlineStr"/>
       <c r="K12" s="2" t="inlineStr"/>
       <c r="L12" s="2" t="inlineStr"/>
+      <c r="M12" s="2" t="inlineStr"/>
+      <c r="N12" s="2" t="inlineStr"/>
+      <c r="O12" s="2" t="inlineStr"/>
+      <c r="P12" s="2" t="inlineStr"/>
+      <c r="Q12" s="2" t="inlineStr"/>
+      <c r="R12" s="2" t="inlineStr"/>
+      <c r="S12" s="2" t="inlineStr"/>
+      <c r="T12" s="2" t="inlineStr"/>
+      <c r="U12" s="2" t="inlineStr"/>
+      <c r="V12" s="2" t="inlineStr"/>
+      <c r="W12" s="2" t="inlineStr"/>
+      <c r="X12" s="2" t="inlineStr"/>
+      <c r="Y12" s="2" t="inlineStr"/>
+      <c r="Z12" s="2" t="inlineStr"/>
+      <c r="AA12" s="2" t="inlineStr"/>
+      <c r="AB12" s="2" t="inlineStr"/>
+      <c r="AC12" s="2" t="inlineStr"/>
+      <c r="AD12" s="2" t="inlineStr"/>
+      <c r="AE12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1124,6 +1424,25 @@
       <c r="J13" s="2" t="inlineStr"/>
       <c r="K13" s="2" t="inlineStr"/>
       <c r="L13" s="2" t="inlineStr"/>
+      <c r="M13" s="2" t="inlineStr"/>
+      <c r="N13" s="2" t="inlineStr"/>
+      <c r="O13" s="2" t="inlineStr"/>
+      <c r="P13" s="2" t="inlineStr"/>
+      <c r="Q13" s="2" t="inlineStr"/>
+      <c r="R13" s="2" t="inlineStr"/>
+      <c r="S13" s="2" t="inlineStr"/>
+      <c r="T13" s="2" t="inlineStr"/>
+      <c r="U13" s="2" t="inlineStr"/>
+      <c r="V13" s="2" t="inlineStr"/>
+      <c r="W13" s="2" t="inlineStr"/>
+      <c r="X13" s="2" t="inlineStr"/>
+      <c r="Y13" s="2" t="inlineStr"/>
+      <c r="Z13" s="2" t="inlineStr"/>
+      <c r="AA13" s="2" t="inlineStr"/>
+      <c r="AB13" s="2" t="inlineStr"/>
+      <c r="AC13" s="2" t="inlineStr"/>
+      <c r="AD13" s="2" t="inlineStr"/>
+      <c r="AE13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1172,6 +1491,25 @@
       <c r="J14" s="2" t="inlineStr"/>
       <c r="K14" s="2" t="inlineStr"/>
       <c r="L14" s="2" t="inlineStr"/>
+      <c r="M14" s="2" t="inlineStr"/>
+      <c r="N14" s="2" t="inlineStr"/>
+      <c r="O14" s="2" t="inlineStr"/>
+      <c r="P14" s="2" t="inlineStr"/>
+      <c r="Q14" s="2" t="inlineStr"/>
+      <c r="R14" s="2" t="inlineStr"/>
+      <c r="S14" s="2" t="inlineStr"/>
+      <c r="T14" s="2" t="inlineStr"/>
+      <c r="U14" s="2" t="inlineStr"/>
+      <c r="V14" s="2" t="inlineStr"/>
+      <c r="W14" s="2" t="inlineStr"/>
+      <c r="X14" s="2" t="inlineStr"/>
+      <c r="Y14" s="2" t="inlineStr"/>
+      <c r="Z14" s="2" t="inlineStr"/>
+      <c r="AA14" s="2" t="inlineStr"/>
+      <c r="AB14" s="2" t="inlineStr"/>
+      <c r="AC14" s="2" t="inlineStr"/>
+      <c r="AD14" s="2" t="inlineStr"/>
+      <c r="AE14" s="2" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1189,7 +1527,7 @@
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>version RTM</t>
+          <t>RTM</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr">
@@ -1220,6 +1558,25 @@
       <c r="J15" s="2" t="inlineStr"/>
       <c r="K15" s="2" t="inlineStr"/>
       <c r="L15" s="2" t="inlineStr"/>
+      <c r="M15" s="2" t="inlineStr"/>
+      <c r="N15" s="2" t="inlineStr"/>
+      <c r="O15" s="2" t="inlineStr"/>
+      <c r="P15" s="2" t="inlineStr"/>
+      <c r="Q15" s="2" t="inlineStr"/>
+      <c r="R15" s="2" t="inlineStr"/>
+      <c r="S15" s="2" t="inlineStr"/>
+      <c r="T15" s="2" t="inlineStr"/>
+      <c r="U15" s="2" t="inlineStr"/>
+      <c r="V15" s="2" t="inlineStr"/>
+      <c r="W15" s="2" t="inlineStr"/>
+      <c r="X15" s="2" t="inlineStr"/>
+      <c r="Y15" s="2" t="inlineStr"/>
+      <c r="Z15" s="2" t="inlineStr"/>
+      <c r="AA15" s="2" t="inlineStr"/>
+      <c r="AB15" s="2" t="inlineStr"/>
+      <c r="AC15" s="2" t="inlineStr"/>
+      <c r="AD15" s="2" t="inlineStr"/>
+      <c r="AE15" s="2" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1237,7 +1594,7 @@
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>version RTM</t>
+          <t>RTM</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr">
@@ -1268,6 +1625,25 @@
       <c r="J16" s="2" t="inlineStr"/>
       <c r="K16" s="2" t="inlineStr"/>
       <c r="L16" s="2" t="inlineStr"/>
+      <c r="M16" s="2" t="inlineStr"/>
+      <c r="N16" s="2" t="inlineStr"/>
+      <c r="O16" s="2" t="inlineStr"/>
+      <c r="P16" s="2" t="inlineStr"/>
+      <c r="Q16" s="2" t="inlineStr"/>
+      <c r="R16" s="2" t="inlineStr"/>
+      <c r="S16" s="2" t="inlineStr"/>
+      <c r="T16" s="2" t="inlineStr"/>
+      <c r="U16" s="2" t="inlineStr"/>
+      <c r="V16" s="2" t="inlineStr"/>
+      <c r="W16" s="2" t="inlineStr"/>
+      <c r="X16" s="2" t="inlineStr"/>
+      <c r="Y16" s="2" t="inlineStr"/>
+      <c r="Z16" s="2" t="inlineStr"/>
+      <c r="AA16" s="2" t="inlineStr"/>
+      <c r="AB16" s="2" t="inlineStr"/>
+      <c r="AC16" s="2" t="inlineStr"/>
+      <c r="AD16" s="2" t="inlineStr"/>
+      <c r="AE16" s="2" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1316,6 +1692,25 @@
       <c r="J17" s="2" t="inlineStr"/>
       <c r="K17" s="2" t="inlineStr"/>
       <c r="L17" s="2" t="inlineStr"/>
+      <c r="M17" s="2" t="inlineStr"/>
+      <c r="N17" s="2" t="inlineStr"/>
+      <c r="O17" s="2" t="inlineStr"/>
+      <c r="P17" s="2" t="inlineStr"/>
+      <c r="Q17" s="2" t="inlineStr"/>
+      <c r="R17" s="2" t="inlineStr"/>
+      <c r="S17" s="2" t="inlineStr"/>
+      <c r="T17" s="2" t="inlineStr"/>
+      <c r="U17" s="2" t="inlineStr"/>
+      <c r="V17" s="2" t="inlineStr"/>
+      <c r="W17" s="2" t="inlineStr"/>
+      <c r="X17" s="2" t="inlineStr"/>
+      <c r="Y17" s="2" t="inlineStr"/>
+      <c r="Z17" s="2" t="inlineStr"/>
+      <c r="AA17" s="2" t="inlineStr"/>
+      <c r="AB17" s="2" t="inlineStr"/>
+      <c r="AC17" s="2" t="inlineStr"/>
+      <c r="AD17" s="2" t="inlineStr"/>
+      <c r="AE17" s="2" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1364,6 +1759,25 @@
       <c r="J18" s="2" t="inlineStr"/>
       <c r="K18" s="2" t="inlineStr"/>
       <c r="L18" s="2" t="inlineStr"/>
+      <c r="M18" s="2" t="inlineStr"/>
+      <c r="N18" s="2" t="inlineStr"/>
+      <c r="O18" s="2" t="inlineStr"/>
+      <c r="P18" s="2" t="inlineStr"/>
+      <c r="Q18" s="2" t="inlineStr"/>
+      <c r="R18" s="2" t="inlineStr"/>
+      <c r="S18" s="2" t="inlineStr"/>
+      <c r="T18" s="2" t="inlineStr"/>
+      <c r="U18" s="2" t="inlineStr"/>
+      <c r="V18" s="2" t="inlineStr"/>
+      <c r="W18" s="2" t="inlineStr"/>
+      <c r="X18" s="2" t="inlineStr"/>
+      <c r="Y18" s="2" t="inlineStr"/>
+      <c r="Z18" s="2" t="inlineStr"/>
+      <c r="AA18" s="2" t="inlineStr"/>
+      <c r="AB18" s="2" t="inlineStr"/>
+      <c r="AC18" s="2" t="inlineStr"/>
+      <c r="AD18" s="2" t="inlineStr"/>
+      <c r="AE18" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>